<commit_message>
crianndo variáveis e teste inicial no cadprev
</commit_message>
<xml_diff>
--- a/plano de amortização.xlsx
+++ b/plano de amortização.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização por aliquotas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633DA04C-D15D-43D2-A787-3C33526F6C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B99FA2E-B449-449E-BD8E-BDBD3DBF7315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="13800" windowHeight="7995" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano_amortizacao vigente" sheetId="2" r:id="rId1"/>
     <sheet name="plano_amortizacao" sheetId="1" r:id="rId2"/>
+    <sheet name="DRAA - Resultados" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="76">
   <si>
     <t>ano</t>
   </si>
@@ -73,13 +74,208 @@
   </si>
   <si>
     <t>tipo_amort_vigente</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Geração Atual</t>
+  </si>
+  <si>
+    <t>Valor Atual dos Salários Futuros</t>
+  </si>
+  <si>
+    <t>ATIVOS GARANTIDORES DOS COMPROMISSOS DO PLANO DE BENEFÍCIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aplicações em Segmento de Renda Fixa - RPPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aplicações em Segmento de Renda Variável - RPPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aplicações em Segmento Imobiliário  - RPPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aplicações em Enquadramento - RPPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Títulos e Valores não Sujeitos ao Enquadramento - RPPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Demais Bens, direitos e ativos</t>
+  </si>
+  <si>
+    <t>PROVISÃO MATEMÁTICA DOS BENEFÍCIOS CONCEDIDOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   VALOR ATUAL DOS BENEFÍCIOS FUTUROS - ENCARGOS DE BENEFÍCIOS CONCEDIDOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Encargos - Aposentadorias Programadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Encargos - Aposentadorias Especiais de Professores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Encargos - Outras Aposentadorias Especiais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Encargos - Aposentadorias por Invalidez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Encargos - Pensões Por Morte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Encargos - Compensação Previdenciária a Pagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   VALOR ATUAL DAS CONTRIBUIÇÕES FUTURAS E COMPENSAÇÕES A RECEBER - BENEFÍCIOS CONCEDIDOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Contribuições Futuras dos Aposentados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Contribuições Futuras dos Pensionistas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios Concedidos - Compensação Previdenciária a Receber</t>
+  </si>
+  <si>
+    <t>PROVISÃO MATEMÁTICA DOS BENEFÍCIOS A CONCEDER:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   VALOR ATUAL DOS BENEFÍCIOS FUTUROS - ENCARGOS DE BENEFÍCIOS A CONCEDER:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Aposentadorias Programadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Aposentadorias Especiais de Professores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Outras Aposentadorias Especiais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Aposentadorias por Invalidez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Pensões Por Morte de Servidores em Atividade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Pensões Por Morte de Aposentados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Outros Benefícios e Auxílios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Encargos - Compensação Previdenciária a Pagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   VALOR ATUAL DAS CONTRIBUIÇÕES FUTURAS E COMPENSAÇÕES A RECEBER - BENEFÍCIOS A CONCEDER:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Contribuições Futuras do Ente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Contribuições Futuras dos Segurados Ativos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Contribuições Futuras dos Aposentados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Contribuições Futuras dos Pensionistas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios a Conceder - Compensação Previdenciária a Receber</t>
+  </si>
+  <si>
+    <t>PROVISÃO MATEMÁTICA PARA COBERTURA DE INSUFICIÊNCIAS FINANCEIRAS ASSEGURADA POR LEI:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Valor Atual do Plano de Amortização do Déficit Atuarial estabelecido em lei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Valor Atual dos Parcelamentos de Débitos Previdenciários</t>
+  </si>
+  <si>
+    <t>RESULTADO ATUARIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Déficit Atuarial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Equilíbrio Atuarial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Superávit Atuarial</t>
+  </si>
+  <si>
+    <t>DESTINAÇÃO DO RESULTADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Provisão de Contingências (até 25% dos Compromissos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Provisão para revisão do plano de custeio (acima 25% dos Compromissos)</t>
+  </si>
+  <si>
+    <t>FUNDOS CONSTITUÍDOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fundo Garantidor de Pensão de Servidor Estruturada em Regime de Repartição de Capitais de Cobertura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fundo Garantidor de Aposentadoria por Invalidez de Servidor Estruturada em Regime de Repartição de Capitais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fundo Garantidor de Benefícios Estruturados em Regime de Repartição Simples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fundo de Oscilação de Riscos dos Benefícios Estruturados em Regime de Capitalização</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fundo de Oscilação de Riscos dos Benefícios Estruturados em Regime de Repartição de Capitais de Cobertura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fundo de Oscilação de Riscos dos Benefícios Estruturados em Regime de Repartição Simples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fundo Administrativo</t>
+  </si>
+  <si>
+    <t>RECEITAS E DESPESAS ESTIMADAS PARA O EXERCÍCIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Total de Receitas Estimadas para o Exercício</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Total de Despesas Estimadas para o Exercício</t>
+  </si>
+  <si>
+    <t>RESULTADO FINANCEIRO ESTIMADO PARA O EXERCÍCIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Déficit Financeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Equilíbrio Financeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Superávit Financeiro</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +300,13 @@
       <sz val="9"/>
       <name val="Maven Pro"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Maven Pro"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +322,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,12 +386,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -202,11 +416,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 8 3" xfId="2" xr:uid="{5F43C3C8-D126-4233-B385-7E7526071F02}"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="3" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,7 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EBBB80-D39B-4C5D-8A0E-1203E2F98462}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -1696,4 +1935,509 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF10D5-ABDD-4F59-8C94-2B7C746ACA7C}">
+  <dimension ref="A1:B62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="104.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11">
+        <v>372140643629</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="12">
+        <v>4693680241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="11">
+        <v>4693680241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="13">
+        <v>6205110301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14">
+        <v>6334824314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="11">
+        <v>362119589.00000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="11">
+        <v>2018465488</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1087043399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2867195838</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="13">
+        <v>129714013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="11">
+        <v>20615686</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="11">
+        <v>109098327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="13">
+        <v>33901773602.000015</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="14">
+        <v>157499181172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="11">
+        <v>74592946760</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="11">
+        <v>58900728662</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="11">
+        <v>4829853727</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="11">
+        <v>19175652023</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="14">
+        <v>123597407569.99998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="11">
+        <v>64560199325.999985</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="11">
+        <v>46114428088</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="11">
+        <v>278414128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="11">
+        <v>44431534</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="11">
+        <v>12599934494</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="14">
+        <v>17731945888.749352</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="11">
+        <v>17731945888.749352</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="15">
+        <v>-176812577.72999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="13"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="12"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="12"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="16">
+        <v>11981116242.09041</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="16">
+        <v>1232488081.4397714</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" s="13"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" s="15">
+        <v>107486281.60650639</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adicionei um script para preenchimento da aba de resultados indo a geração futura
</commit_message>
<xml_diff>
--- a/plano de amortização.xlsx
+++ b/plano de amortização.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B99FA2E-B449-449E-BD8E-BDBD3DBF7315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C7CEC5-A6B8-46B5-8AE4-F2F407A85496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="13800" windowHeight="7995" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano_amortizacao vigente" sheetId="2" r:id="rId1"/>
-    <sheet name="plano_amortizacao" sheetId="1" r:id="rId2"/>
+    <sheet name="plano_amortizacao_suplementar" sheetId="1" r:id="rId2"/>
     <sheet name="DRAA - Resultados" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
     <t>ano</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Gerações Futuras</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,7 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -438,6 +441,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -726,10 +732,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -739,7 +745,7 @@
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>2021</v>
       </c>
@@ -777,7 +783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2022</v>
       </c>
@@ -792,7 +798,7 @@
         <v>47.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2023</v>
       </c>
@@ -807,7 +813,7 @@
         <v>47.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>2024</v>
       </c>
@@ -822,7 +828,7 @@
         <v>52.459999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2025</v>
       </c>
@@ -837,7 +843,7 @@
         <v>53.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2026</v>
       </c>
@@ -852,7 +858,7 @@
         <v>53.741000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>2027</v>
       </c>
@@ -867,7 +873,7 @@
         <v>54.379999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>2028</v>
       </c>
@@ -882,7 +888,7 @@
         <v>55.02</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>2029</v>
       </c>
@@ -897,7 +903,7 @@
         <v>55.65</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>2030</v>
       </c>
@@ -912,7 +918,7 @@
         <v>56.289999999999992</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>2031</v>
       </c>
@@ -927,7 +933,7 @@
         <v>56.93</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>2032</v>
       </c>
@@ -942,7 +948,7 @@
         <v>57.57</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>2033</v>
       </c>
@@ -957,7 +963,7 @@
         <v>58.209999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>2034</v>
       </c>
@@ -972,7 +978,7 @@
         <v>58.84</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>2035</v>
       </c>
@@ -987,7 +993,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>2036</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>2037</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>2038</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>2039</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>2040</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>2041</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>2042</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>2043</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>2044</v>
       </c>
@@ -1122,7 +1128,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>2045</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>2046</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>2047</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>2048</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>2049</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>2050</v>
       </c>
@@ -1212,7 +1218,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>2051</v>
       </c>
@@ -1227,7 +1233,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>2052</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>2053</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>2054</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>59.48</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>2055</v>
       </c>
@@ -1296,9 +1302,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -1310,7 +1318,7 @@
     <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>2022</v>
       </c>
@@ -1353,7 +1361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2023</v>
       </c>
@@ -1370,7 +1378,7 @@
         <v>2411749084.8100009</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2024</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>2435866575.6581011</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2025</v>
       </c>
@@ -1404,7 +1412,7 @@
         <v>2460225241.4146824</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2026</v>
       </c>
@@ -1421,7 +1429,7 @@
         <v>2484827493.8288288</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>2027</v>
       </c>
@@ -1438,7 +1446,7 @@
         <v>2509675768.7671175</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2028</v>
       </c>
@@ -1455,7 +1463,7 @@
         <v>2534772526.4547882</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>2029</v>
       </c>
@@ -1472,7 +1480,7 @@
         <v>2560120251.7193365</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>2030</v>
       </c>
@@ -1489,7 +1497,7 @@
         <v>2585721454.2365303</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>2031</v>
       </c>
@@ -1506,7 +1514,7 @@
         <v>2611578668.7788954</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>2032</v>
       </c>
@@ -1523,7 +1531,7 @@
         <v>2637694455.4666839</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>2033</v>
       </c>
@@ -1540,7 +1548,7 @@
         <v>2664071400.0213509</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2034</v>
       </c>
@@ -1557,7 +1565,7 @@
         <v>2690712114.0215645</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2035</v>
       </c>
@@ -1574,7 +1582,7 @@
         <v>2717619235.1617804</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>2036</v>
       </c>
@@ -1591,7 +1599,7 @@
         <v>2744795427.5133977</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>2037</v>
       </c>
@@ -1608,7 +1616,7 @@
         <v>2772243381.7885323</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>2038</v>
       </c>
@@ -1625,7 +1633,7 @@
         <v>2799965815.6064177</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2039</v>
       </c>
@@ -1642,7 +1650,7 @@
         <v>2827965473.7624822</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>2040</v>
       </c>
@@ -1659,7 +1667,7 @@
         <v>2856245128.5001063</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>2041</v>
       </c>
@@ -1676,7 +1684,7 @@
         <v>2884807579.7851076</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>2042</v>
       </c>
@@ -1693,7 +1701,7 @@
         <v>2913655655.5829582</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2043</v>
       </c>
@@ -1710,7 +1718,7 @@
         <v>2942792212.1387887</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2044</v>
       </c>
@@ -1727,7 +1735,7 @@
         <v>2972220134.2601762</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>2045</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>3001942335.6027784</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>2046</v>
       </c>
@@ -1761,7 +1769,7 @@
         <v>3031961758.958807</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>2047</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>3062281376.5483947</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>2048</v>
       </c>
@@ -1795,7 +1803,7 @@
         <v>3092904190.3138776</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>2049</v>
       </c>
@@ -1812,7 +1820,7 @@
         <v>3123833232.2170162</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>2050</v>
       </c>
@@ -1829,7 +1837,7 @@
         <v>3155071564.539187</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>2051</v>
       </c>
@@ -1846,7 +1854,7 @@
         <v>3186622280.1845794</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>2052</v>
       </c>
@@ -1863,7 +1871,7 @@
         <v>3218488502.986424</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>2053</v>
       </c>
@@ -1880,7 +1888,7 @@
         <v>3250673388.0162892</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>2054</v>
       </c>
@@ -1897,7 +1905,7 @@
         <v>3283180121.896452</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>2055</v>
       </c>
@@ -1914,7 +1922,7 @@
         <v>3316011923.1154165</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>2056</v>
       </c>
@@ -1939,502 +1947,656 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF10D5-ABDD-4F59-8C94-2B7C746ACA7C}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="104.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="11">
         <v>372140643629</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="10">
+        <v>111184810</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="12">
         <v>4693680241</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="11">
+        <v>111111111</v>
+      </c>
+      <c r="C4" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="11">
+        <v>22222222</v>
+      </c>
+      <c r="C5" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="11">
+        <v>3333333333333</v>
+      </c>
+      <c r="C6" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.25" customHeight="1">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="11">
+        <v>4444444444444</v>
+      </c>
+      <c r="C7" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="11">
+        <v>55555555555555</v>
+      </c>
+      <c r="C8" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="11">
-        <v>4693680241</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>5689742597</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="13">
         <v>6205110301</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="14">
         <v>6334824314</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="11">
         <v>362119589.00000006</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="11">
         <v>2018465488</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="11">
+        <v>1111111111</v>
+      </c>
+      <c r="C14" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="11">
         <v>1087043399</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="11">
         <v>2867195838</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="11">
+        <v>22222222222</v>
+      </c>
+      <c r="C17" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="13">
         <v>129714013</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="11">
         <v>20615686</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="11">
         <v>109098327</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="11">
+        <v>11111111111111</v>
+      </c>
+      <c r="C21" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="13">
         <v>33901773602.000015</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="14">
         <v>157499181172</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="11">
         <v>74592946760</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="10">
+        <v>11111111111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="11">
         <v>58900728662</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="10">
+        <v>222222222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="11">
         <v>4829853727</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="10">
+        <v>3333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>1111111111111</v>
+      </c>
+      <c r="C27" s="10">
+        <v>4444444444</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>222222222222</v>
+      </c>
+      <c r="C28" s="10">
+        <v>55555555555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="11">
         <v>19175652023</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="10">
+        <v>66666666666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>3333333333</v>
+      </c>
+      <c r="C30" s="10">
+        <v>77777777777</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>4444444444444</v>
+      </c>
+      <c r="C31" s="10">
+        <v>88888888888</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="14">
         <v>123597407569.99998</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="11">
         <v>64560199325.999985</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="10">
+        <v>11111111111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="11">
         <v>46114428088</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" s="10">
+        <v>22222222222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B35" s="11">
         <v>278414128</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="10">
+        <v>3333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B36" s="11">
         <v>44431534</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" s="10">
+        <v>4444444444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="11">
         <v>12599934494</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="10">
+        <v>5555555555</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B38" s="14">
         <v>17731945888.749352</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B39" s="11">
         <v>17731945888.749352</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" s="10">
+        <v>11111111111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B40" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>111111111111111</v>
+      </c>
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B41" s="15"/>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B42" s="15">
         <v>-176812577.72999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>57</v>
       </c>
       <c r="B45" s="13"/>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B46" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>898998089</v>
+      </c>
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>78978562623</v>
+      </c>
+      <c r="C47" s="13"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B48" s="12"/>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" s="13"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B49" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>999999999</v>
+      </c>
+      <c r="C49" s="13"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B50" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>111111111111111</v>
+      </c>
+      <c r="C50" s="13"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B51" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>222222222222222</v>
+      </c>
+      <c r="C51" s="13"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B52" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>33333333333</v>
+      </c>
+      <c r="C52" s="13"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B53" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>4444444444444</v>
+      </c>
+      <c r="C53" s="13"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B54" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>555555555555</v>
+      </c>
+      <c r="C54" s="13"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B55" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>7897484546</v>
+      </c>
+      <c r="C55" s="13"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="12"/>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" s="13"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B57" s="16">
         <v>11981116242.09041</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B58" s="16">
         <v>1232488081.4397714</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" s="13"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B59" s="13"/>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" s="13"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" s="13"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" s="13"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B62" s="15">
         <v>107486281.60650639</v>
+      </c>
+      <c r="C62" s="13"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <f>1736-1546</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <f>1729-1546</f>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script de comparativo fr informações
</commit_message>
<xml_diff>
--- a/plano de amortização.xlsx
+++ b/plano de amortização.xlsx
@@ -8,15 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C7CEC5-A6B8-46B5-8AE4-F2F407A85496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B7AEA2-24F5-4B86-AD5D-761A33A17E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano_amortizacao vigente" sheetId="2" r:id="rId1"/>
     <sheet name="plano_amortizacao_suplementar" sheetId="1" r:id="rId2"/>
     <sheet name="DRAA - Resultados" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparativo" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="Método">'[1]Resultados Atuariais'!$B$16</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="119">
   <si>
     <t>ano</t>
   </si>
@@ -269,6 +276,132 @@
   </si>
   <si>
     <t>Gerações Futuras</t>
+  </si>
+  <si>
+    <t>BASE NORMATIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   PLANO DE CUSTEIO VIGENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Contribuição Normal - Ente Federativo</t>
+  </si>
+  <si>
+    <t>BASE CADASTRAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ESTATÍSTICAS DA POPULAÇÃO COBERTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Quantidade de Segurados Ativos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Quantidade de Aposentados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Quantidade de Pensionistas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Média da Base de Cálculo dos Segurados Ativos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Média do Valor do Beneficio dos Aposentados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Média do Valor do Benefícios dos Pensionistas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Idade Média dos Segurados Ativos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Idade Média dos Aposentados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Idade Média dos Pensionistas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Idade Média Projetada Para Aposentadoria</t>
+  </si>
+  <si>
+    <t>BASE TÉCNICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   REGIMES E MÉTODOS DE FINANCIAMENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Método de Financiamento Adotado</t>
+  </si>
+  <si>
+    <t>RESULTADOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   VALORES DOS COMPROMISSOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Ativos Garantidores dos Compromissos do Plano de Benefícios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Valor Atual dos Benefícios Futuros - Benefícios Concedidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Valor Atual das Contribuições Futuras - Benefícios Concedidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Reserva Matemática dos Benefícios Concedidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Valor Atual dos Benefícios Futuros - Benefícios a Conceder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Valor Atual das Contribuições Futuras - Benefícios a Conceder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Reserva Matemática dos Benefícios a Conceder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Valor Atual da Compensação Financeira a Receber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Valor Atual da Compensação Financeira a Pagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Resultado Atuarial</t>
+  </si>
+  <si>
+    <t>CUSTO NORMAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   CUSTO ANUAL PREVISTO (% SOBRE BASE DE CONTRIBUIÇÃO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios em Regime de Capitalização (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios em Regime de Repartição de Capitais de Cobertura (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Benefícios em Regime de Repartição Simples (%)</t>
+  </si>
+  <si>
+    <t>ALÍQUOTAS DE CUSTEIO NORMAL DEFINIDAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Ente Federativo - Contribuição Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Taxa de Administração</t>
+  </si>
+  <si>
+    <t>Ano1</t>
+  </si>
+  <si>
+    <t>Ano2</t>
+  </si>
+  <si>
+    <t>Ano3</t>
+  </si>
+  <si>
+    <t>AGREGADO 2</t>
   </si>
 </sst>
 </file>
@@ -464,6 +597,170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Caixa de diálogo2"/>
+      <sheetName val="Ref_Colunas"/>
+      <sheetName val="TABUAS"/>
+      <sheetName val="ÍNDICES"/>
+      <sheetName val="Reajustes"/>
+      <sheetName val="Duration Passivo"/>
+      <sheetName val="Gráfico1"/>
+      <sheetName val="Macro Word (2)"/>
+      <sheetName val="COMANDOS"/>
+      <sheetName val="Informações sobre o Banco"/>
+      <sheetName val="Localizar"/>
+      <sheetName val="Dados"/>
+      <sheetName val="Listinhas"/>
+      <sheetName val="Aliq Progres"/>
+      <sheetName val="Parametros Elegibilidade EC103"/>
+      <sheetName val="Parcelamentos"/>
+      <sheetName val="Despesas Administrativas"/>
+      <sheetName val="Ativos Critica"/>
+      <sheetName val="Aposentados Critica"/>
+      <sheetName val="Pensionistas Critica"/>
+      <sheetName val="Ativos"/>
+      <sheetName val="Inativos"/>
+      <sheetName val="Pensionistas"/>
+      <sheetName val="PensionistasCotas"/>
+      <sheetName val="Estatísticas ATIVOS"/>
+      <sheetName val="Projeção Ativos PROG"/>
+      <sheetName val="Projeção Ativos ESP PROFESSOR"/>
+      <sheetName val="Projeção Ativos ESP DEFICIENTE"/>
+      <sheetName val="Projeção Ativos ESP RISCO"/>
+      <sheetName val="Projeção Ativos ESP INSALUBRE"/>
+      <sheetName val="Projeção Ativos RCC"/>
+      <sheetName val="Teste Regressão Casados"/>
+      <sheetName val="Projeção de Massa IEN"/>
+      <sheetName val="Estatisticas Aposentados"/>
+      <sheetName val="Projeção Aposentados"/>
+      <sheetName val="Estatisticas Pensionistas"/>
+      <sheetName val="Projeção Pensionistas"/>
+      <sheetName val="Negociação Fluxos"/>
+      <sheetName val="Hipoteses"/>
+      <sheetName val="Checklist"/>
+      <sheetName val="MÉTODOS progressiva"/>
+      <sheetName val="Resultados"/>
+      <sheetName val="BD TABUAS"/>
+      <sheetName val="CustoSuplementar"/>
+      <sheetName val="LDA"/>
+      <sheetName val="Análise de Sensibilidade"/>
+      <sheetName val="RELATÓRIO"/>
+      <sheetName val="Macro Word"/>
+      <sheetName val="Listas"/>
+      <sheetName val="Rec Des proj exercicio - Atual"/>
+      <sheetName val="RELATÓRIO ref Word"/>
+      <sheetName val="Resultados Atuariais"/>
+      <sheetName val="Gráfico2"/>
+      <sheetName val="Gráfico3"/>
+      <sheetName val="Projeções - sem GF"/>
+      <sheetName val="Flx CX vigente - LINEAR"/>
+      <sheetName val="Flx CX vigente - PROGRESSIVA"/>
+      <sheetName val="Quadros da Reav COMPARATIVO"/>
+      <sheetName val="Registros Contábeis"/>
+      <sheetName val="Crescimento Salarial - PREV"/>
+      <sheetName val="DRAA Negociação"/>
+      <sheetName val="DRAA Órgãos_CNPJ"/>
+      <sheetName val="DRAA Base Técnica"/>
+      <sheetName val="DRAA Resultados"/>
+      <sheetName val="DRAA Estatisticas"/>
+      <sheetName val="DRAA Estatisticas PREV COMPL"/>
+      <sheetName val="DRAA Flx_CIVIL_PREV_GA"/>
+      <sheetName val="DRAA FLUXO x DRAA PREV"/>
+      <sheetName val="Projeção Ativos PROG IEN"/>
+      <sheetName val="Projeção Ativos ESP PROF IEN"/>
+      <sheetName val="Projeção Ativos ESP DEFIC IEN"/>
+      <sheetName val="Projeção Ativos ESP RISCO IEN"/>
+      <sheetName val="Projeção Ativos ESP INSALUB IEN"/>
+      <sheetName val="Prévia Resultados"/>
+      <sheetName val="PlanAuxiliar"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51">
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>AGREGADO 2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1949,7 +2246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF10D5-ABDD-4F59-8C94-2B7C746ACA7C}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
@@ -2602,4 +2899,559 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F764EF3B-304D-4F9A-AF09-04DC8A7C5C52}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2600</v>
+      </c>
+      <c r="C4" s="10">
+        <f>B4*1.01</f>
+        <v>2626</v>
+      </c>
+      <c r="D4" s="10">
+        <f>C4*1.01</f>
+        <v>2652.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="10">
+        <v>11111</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" ref="C7:D16" si="0">B7*1.01</f>
+        <v>11222.11</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>11334.331100000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2222</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" si="0"/>
+        <v>2244.2199999999998</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>2266.6621999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="10">
+        <v>3333</v>
+      </c>
+      <c r="C9" s="10">
+        <f t="shared" si="0"/>
+        <v>3366.33</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="0"/>
+        <v>3399.9933000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C10" s="10">
+        <f t="shared" si="0"/>
+        <v>4488.4399999999996</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="0"/>
+        <v>4533.3243999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="10">
+        <v>5555</v>
+      </c>
+      <c r="C11" s="10">
+        <f t="shared" si="0"/>
+        <v>5610.55</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="0"/>
+        <v>5666.6554999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="10">
+        <v>6666</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="0"/>
+        <v>6732.66</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="0"/>
+        <v>6799.9866000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="11">
+        <v>7777</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="0"/>
+        <v>7854.77</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
+        <v>7933.3177000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="11">
+        <v>8888</v>
+      </c>
+      <c r="C14" s="11">
+        <f t="shared" si="0"/>
+        <v>8976.8799999999992</v>
+      </c>
+      <c r="D14" s="11">
+        <f t="shared" si="0"/>
+        <v>9066.648799999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="11">
+        <v>9999</v>
+      </c>
+      <c r="C15" s="11">
+        <f t="shared" si="0"/>
+        <v>10098.99</v>
+      </c>
+      <c r="D15" s="11">
+        <f t="shared" si="0"/>
+        <v>10199.9799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1010</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" si="0"/>
+        <v>1020.1</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
+        <v>1030.3009999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="9" t="str">
+        <f>Método</f>
+        <v>AGREGADO 2</v>
+      </c>
+      <c r="D19" s="9" t="str">
+        <f>Método</f>
+        <v>AGREGADO 2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="10">
+        <v>615548334</v>
+      </c>
+      <c r="C22" s="10">
+        <f t="shared" ref="C22:D31" si="1">B22*1.01</f>
+        <v>621703817.34000003</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" si="1"/>
+        <v>627920855.51340008</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="10">
+        <v>20127686644</v>
+      </c>
+      <c r="C23" s="10">
+        <f t="shared" si="1"/>
+        <v>20328963510.439999</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="1"/>
+        <v>20532253145.544399</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="10">
+        <v>44331443</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" si="1"/>
+        <v>44774757.43</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="1"/>
+        <v>45222505.004299998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="10">
+        <v>20083355201</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" si="1"/>
+        <v>20284188753.009998</v>
+      </c>
+      <c r="D25" s="10">
+        <f t="shared" si="1"/>
+        <v>20487030640.5401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="10">
+        <v>18456662527</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="1"/>
+        <v>18641229152.27</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" si="1"/>
+        <v>18827641443.792702</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="10">
+        <v>7533249022</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="1"/>
+        <v>7608581512.2200003</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="1"/>
+        <v>7684667327.3422003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="10">
+        <v>10923413505</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="1"/>
+        <v>11032647640.049999</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="1"/>
+        <v>11142974116.450499</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1396386982</v>
+      </c>
+      <c r="C29" s="10">
+        <f t="shared" si="1"/>
+        <v>1410350851.8199999</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" si="1"/>
+        <v>1424454360.3381999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="10">
+        <v>88484877</v>
+      </c>
+      <c r="C30" s="10">
+        <f t="shared" si="1"/>
+        <v>89369725.769999996</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="1"/>
+        <v>90263423.027699992</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="10">
+        <v>28994833390</v>
+      </c>
+      <c r="C31" s="10">
+        <f t="shared" si="1"/>
+        <v>29284781723.900002</v>
+      </c>
+      <c r="D31" s="10">
+        <f t="shared" si="1"/>
+        <v>29577629541.139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="10">
+        <v>3539.6807377431933</v>
+      </c>
+      <c r="C34" s="10">
+        <f t="shared" ref="C34:D36" si="2">B34*1.01</f>
+        <v>3575.077545120625</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="2"/>
+        <v>3610.8283205718312</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="10">
+        <v>360.31926300187229</v>
+      </c>
+      <c r="C35" s="10">
+        <f t="shared" si="2"/>
+        <v>363.92245563189101</v>
+      </c>
+      <c r="D35" s="10">
+        <f t="shared" si="2"/>
+        <v>367.56168018820995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="10">
+        <v>3539.6807377431933</v>
+      </c>
+      <c r="C36" s="11">
+        <f t="shared" si="2"/>
+        <v>3575.077545120625</v>
+      </c>
+      <c r="D36" s="11">
+        <f t="shared" si="2"/>
+        <v>3610.8283205718312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="10">
+        <v>2400</v>
+      </c>
+      <c r="C38" s="10">
+        <f t="shared" ref="C38:D39" si="3">B38*1.01</f>
+        <v>2424</v>
+      </c>
+      <c r="D38" s="10">
+        <f t="shared" si="3"/>
+        <v>2448.2400000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="10">
+        <v>200</v>
+      </c>
+      <c r="C39" s="10">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
+      <c r="D39" s="10">
+        <f t="shared" si="3"/>
+        <v>204.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
preenchimento de comparativo previsto/executado
</commit_message>
<xml_diff>
--- a/plano de amortização.xlsx
+++ b/plano de amortização.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA22B968-28BC-4733-8DA1-8C27124447D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FCAB5-2549-43DB-8807-8828FB476494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5731,7 +5731,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5900,7 +5900,7 @@
         <v>249</v>
       </c>
       <c r="B14" s="24">
-        <v>4846118564</v>
+        <v>1111111</v>
       </c>
       <c r="C14" s="24">
         <v>6057648205</v>
@@ -5912,7 +5912,7 @@
         <v>250</v>
       </c>
       <c r="B15" s="24">
-        <v>484484164</v>
+        <v>2222222</v>
       </c>
       <c r="C15" s="24">
         <v>605605205</v>
@@ -5924,7 +5924,7 @@
         <v>251</v>
       </c>
       <c r="B16" s="24">
-        <v>48456486464</v>
+        <v>3333333</v>
       </c>
       <c r="C16" s="24">
         <v>60570608080</v>
@@ -5936,7 +5936,7 @@
         <v>252</v>
       </c>
       <c r="B17" s="24">
-        <v>4849159648</v>
+        <v>4444444</v>
       </c>
       <c r="C17" s="24">
         <v>6061449560</v>
@@ -5948,7 +5948,7 @@
         <v>253</v>
       </c>
       <c r="B18" s="24">
-        <v>48944894231</v>
+        <v>5555555</v>
       </c>
       <c r="C18" s="24">
         <v>6116617789</v>
@@ -5960,7 +5960,7 @@
         <v>254</v>
       </c>
       <c r="B19" s="24">
-        <v>895688656</v>
+        <v>6666666</v>
       </c>
       <c r="C19" s="24">
         <v>1119610820</v>
@@ -5972,7 +5972,7 @@
         <v>255</v>
       </c>
       <c r="B20" s="24">
-        <v>96786324245</v>
+        <v>7777777</v>
       </c>
       <c r="C20" s="24">
         <v>18290530625</v>
@@ -5984,7 +5984,7 @@
         <v>256</v>
       </c>
       <c r="B21" s="24">
-        <v>686565</v>
+        <v>8888888</v>
       </c>
       <c r="C21" s="24">
         <v>858206.25</v>
@@ -5996,7 +5996,7 @@
         <v>257</v>
       </c>
       <c r="B22" s="24">
-        <v>9898956</v>
+        <v>999999</v>
       </c>
       <c r="C22" s="24">
         <v>12373695</v>
@@ -6008,7 +6008,7 @@
         <v>258</v>
       </c>
       <c r="B23" s="24">
-        <v>298568</v>
+        <v>10101010</v>
       </c>
       <c r="C23" s="24">
         <v>373210</v>
@@ -6020,7 +6020,7 @@
         <v>259</v>
       </c>
       <c r="B24" s="24">
-        <v>3587979</v>
+        <v>1111111111</v>
       </c>
       <c r="C24" s="24">
         <v>4484973.75</v>
@@ -6032,7 +6032,7 @@
         <v>260</v>
       </c>
       <c r="B25" s="24">
-        <v>878456185</v>
+        <v>121211222</v>
       </c>
       <c r="C25" s="24">
         <v>1098070231.25</v>
@@ -6044,7 +6044,7 @@
         <v>261</v>
       </c>
       <c r="B26" s="24">
-        <v>3968995</v>
+        <v>13131313</v>
       </c>
       <c r="C26" s="24">
         <v>4961243.75</v>
@@ -6056,7 +6056,7 @@
         <v>262</v>
       </c>
       <c r="B27" s="24">
-        <v>68458545</v>
+        <v>1414141414</v>
       </c>
       <c r="C27" s="24">
         <v>85573181.25</v>
@@ -6068,7 +6068,7 @@
         <v>263</v>
       </c>
       <c r="B28" s="24">
-        <v>878654654</v>
+        <v>15151515155</v>
       </c>
       <c r="C28" s="24">
         <v>1098318317.5</v>
@@ -6080,7 +6080,7 @@
         <v>264</v>
       </c>
       <c r="B29" s="24">
-        <v>748765156</v>
+        <v>161616161</v>
       </c>
       <c r="C29" s="24">
         <v>935956445</v>

</xml_diff>

<commit_message>
adicionado script do cadastro de ente e UG
</commit_message>
<xml_diff>
--- a/plano de amortização.xlsx
+++ b/plano de amortização.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FCAB5-2549-43DB-8807-8828FB476494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F05A2-C297-4339-9235-014C4732C9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano_amortizacao vigente" sheetId="2" r:id="rId1"/>
@@ -20,9 +20,13 @@
     <sheet name="Órgãos_Entidades" sheetId="6" r:id="rId5"/>
     <sheet name="Modelo DRAA Precificador" sheetId="5" r:id="rId6"/>
     <sheet name="Comparativo proj-exe" sheetId="7" r:id="rId7"/>
+    <sheet name="Ente" sheetId="8" r:id="rId8"/>
+    <sheet name="UG" sheetId="9" r:id="rId9"/>
+    <sheet name="Atuário" sheetId="10" r:id="rId10"/>
+    <sheet name="Composição de massa" sheetId="11" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Modelo DRAA Precificador'!$A$1:$N$11</definedName>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="369">
   <si>
     <t>ano</t>
   </si>
@@ -862,6 +866,300 @@
   </si>
   <si>
     <t>Projetado</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Bairro</t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Cod_cargo</t>
+  </si>
+  <si>
+    <t>Complemento cargo</t>
+  </si>
+  <si>
+    <t>Dt inicio gestão</t>
+  </si>
+  <si>
+    <t>E-mail ente</t>
+  </si>
+  <si>
+    <t>E-mail representante</t>
+  </si>
+  <si>
+    <t>Rua Daura Saraiva</t>
+  </si>
+  <si>
+    <t>n° 591</t>
+  </si>
+  <si>
+    <t>jardim</t>
+  </si>
+  <si>
+    <t>weuqiuweqio@gmail.com</t>
+  </si>
+  <si>
+    <t>jewiojropwe</t>
+  </si>
+  <si>
+    <t>cargo</t>
+  </si>
+  <si>
+    <t>Prefeito</t>
+  </si>
+  <si>
+    <t>Governador</t>
+  </si>
+  <si>
+    <t>Secretário</t>
+  </si>
+  <si>
+    <t>Tesoureiro</t>
+  </si>
+  <si>
+    <t>Vice-prefeito</t>
+  </si>
+  <si>
+    <t>da economia</t>
+  </si>
+  <si>
+    <t>da cultura</t>
+  </si>
+  <si>
+    <t>tjrtjreo@gmail.com</t>
+  </si>
+  <si>
+    <t>natureza juridica</t>
+  </si>
+  <si>
+    <t>Artarquia</t>
+  </si>
+  <si>
+    <t>Fundação de direito público</t>
+  </si>
+  <si>
+    <t>Órgão da adm direta</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>cod_cargo</t>
+  </si>
+  <si>
+    <t>Adm</t>
+  </si>
+  <si>
+    <t>Diretor</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>Gestor</t>
+  </si>
+  <si>
+    <t>Membro</t>
+  </si>
+  <si>
+    <t>Presidente</t>
+  </si>
+  <si>
+    <t>Superintendente</t>
+  </si>
+  <si>
+    <t>Vice-presidente</t>
+  </si>
+  <si>
+    <t>dt_inicio gestao</t>
+  </si>
+  <si>
+    <t>Denominação</t>
+  </si>
+  <si>
+    <t>Entidade Certificadora</t>
+  </si>
+  <si>
+    <t>Validade da Certificação</t>
+  </si>
+  <si>
+    <t>Cod_vinculo</t>
+  </si>
+  <si>
+    <t>MTE</t>
+  </si>
+  <si>
+    <t>IBA</t>
+  </si>
+  <si>
+    <t>Nome_empresa</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Cod_UF</t>
+  </si>
+  <si>
+    <t>CIBA</t>
+  </si>
+  <si>
+    <t>Infor_ad</t>
+  </si>
+  <si>
+    <t>cod_segreg_militar</t>
+  </si>
+  <si>
+    <t>cod_sereg_civil</t>
+  </si>
+  <si>
+    <t>mant_tesouro_civil</t>
+  </si>
+  <si>
+    <t>mant_tesouro_militar</t>
+  </si>
+  <si>
+    <t>Cod_prev_compl</t>
+  </si>
+  <si>
+    <t>09405591452</t>
+  </si>
+  <si>
+    <t>01/10/1999</t>
+  </si>
+  <si>
+    <t>ao lado da igreja</t>
+  </si>
+  <si>
+    <t>ruweioruweo@gmail.com</t>
+  </si>
+  <si>
+    <t>Chicao</t>
+  </si>
+  <si>
+    <t>ruweioruo@gmail.com</t>
+  </si>
+  <si>
+    <t>E-mail_UG</t>
+  </si>
+  <si>
+    <t>Telefone_UG</t>
+  </si>
+  <si>
+    <t>Telefone_REP</t>
+  </si>
+  <si>
+    <t>E-mail_REP</t>
+  </si>
+  <si>
+    <t>primo do mão do tio do vice-prefeito</t>
+  </si>
+  <si>
+    <t>cod_norma</t>
+  </si>
+  <si>
+    <t>norma</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>lei</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Decreto</t>
+  </si>
+  <si>
+    <t>Portaria</t>
+  </si>
+  <si>
+    <t>Resolução</t>
+  </si>
+  <si>
+    <t>num_norma</t>
+  </si>
+  <si>
+    <t>dt_norma</t>
+  </si>
+  <si>
+    <t>dispositivo_norma</t>
+  </si>
+  <si>
+    <t>n_repres_ente</t>
+  </si>
+  <si>
+    <t>n_repres_seg</t>
+  </si>
+  <si>
+    <t>outros</t>
+  </si>
+  <si>
+    <t>CPF_deliberativo</t>
+  </si>
+  <si>
+    <t>Telefone_delib</t>
+  </si>
+  <si>
+    <t>E-mail_delib</t>
+  </si>
+  <si>
+    <t>Dt_inicio_mandato</t>
+  </si>
+  <si>
+    <t>02/02/2000</t>
+  </si>
+  <si>
+    <t>da oficina</t>
+  </si>
+  <si>
+    <t>ruweiurwoe@gmail.com</t>
+  </si>
+  <si>
+    <t>complemento cargo_UG</t>
+  </si>
+  <si>
+    <t>Nome_UG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod_natureza </t>
+  </si>
+  <si>
+    <t>06347458675</t>
+  </si>
+  <si>
+    <t>05/05/2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonho </t>
+  </si>
+  <si>
+    <t>Vendedor de inhame</t>
+  </si>
+  <si>
+    <t>31/12/2021</t>
   </si>
 </sst>
 </file>
@@ -872,7 +1170,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,6 +1222,14 @@
       <color rgb="FFF8F8F2"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1043,15 +1349,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1120,8 +1427,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="Hiperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Moeda 2" xfId="5" xr:uid="{87304AA8-01AF-412A-AB91-CB4511961F90}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10 2 2" xfId="4" xr:uid="{DA7B93F6-CC75-46B5-A74E-8B8E710ACC31}"/>
@@ -2141,6 +2456,125 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4D80C-8621-48E7-94DF-8C2C1D847455}">
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I1" t="s">
+        <v>318</v>
+      </c>
+      <c r="J1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" t="s">
+        <v>319</v>
+      </c>
+      <c r="L1" t="s">
+        <v>271</v>
+      </c>
+      <c r="M1" t="s">
+        <v>272</v>
+      </c>
+      <c r="N1" t="s">
+        <v>320</v>
+      </c>
+      <c r="O1" t="s">
+        <v>321</v>
+      </c>
+      <c r="P1" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>276</v>
+      </c>
+      <c r="R1" t="s">
+        <v>275</v>
+      </c>
+      <c r="S1" t="s">
+        <v>322</v>
+      </c>
+      <c r="T1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC23F32-023E-4679-8D32-C792213F62D3}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
@@ -2792,8 +3226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF10D5-ABDD-4F59-8C94-2B7C746ACA7C}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,7 +6164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737DF4F8-5AC6-4CD3-A777-EBE20E8E4EAD}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -6139,4 +6573,836 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1491B68-B113-4854-8907-E7E5C981C4E4}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" t="s">
+        <v>279</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="K1" t="s">
+        <v>280</v>
+      </c>
+      <c r="L1" t="s">
+        <v>281</v>
+      </c>
+      <c r="M1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2">
+        <v>58113410</v>
+      </c>
+      <c r="E2">
+        <v>83998630647</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="H2" t="s">
+        <v>288</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="K2" t="s">
+        <v>295</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="D3" s="20">
+        <v>58113410</v>
+      </c>
+      <c r="E3" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="D4" s="20">
+        <v>58113410</v>
+      </c>
+      <c r="E4" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" s="20">
+        <v>58113410</v>
+      </c>
+      <c r="E5" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="K5" t="s">
+        <v>296</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" s="20">
+        <v>58113410</v>
+      </c>
+      <c r="E6" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="M6" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{084E0C5E-DAE1-4B75-8F89-FAD5CD9F6CB0}"/>
+    <hyperlink ref="M3:M6" r:id="rId2" display="tjrtjreo@gmail.com" xr:uid="{32AD2657-42AC-4C51-A8E9-2C98114603DC}"/>
+    <hyperlink ref="F2" r:id="rId3" display="tjrtjreo@gmail.com" xr:uid="{E8B2D925-9EB9-4EB6-97B1-64D5241A5B2A}"/>
+    <hyperlink ref="F3" r:id="rId4" display="tjrtjreo@gmail.com" xr:uid="{5890A241-2DED-4905-B4AE-02337E844B6D}"/>
+    <hyperlink ref="F4" r:id="rId5" display="tjrtjreo@gmail.com" xr:uid="{9879A88F-6C31-4A8A-8A90-ED4AEAE5CD5D}"/>
+    <hyperlink ref="F5" r:id="rId6" display="tjrtjreo@gmail.com" xr:uid="{E3BDE2FE-64B0-4D2A-84B8-3789B5D9789C}"/>
+    <hyperlink ref="F6" r:id="rId7" display="tjrtjreo@gmail.com" xr:uid="{92136D6B-29FA-4488-97CE-2EE69CD83340}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB190852-2510-45CC-A5C2-C7FDFE63385C}">
+  <dimension ref="A1:AI11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.28515625" style="20" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>363</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>341</v>
+      </c>
+      <c r="V1" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="W1" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="X1" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="Y1" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="Z1" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="AA1" s="30" t="s">
+        <v>353</v>
+      </c>
+      <c r="AB1" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="AC1" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="AD1" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE1" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="AF1" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="AG1" s="30" t="s">
+        <v>355</v>
+      </c>
+      <c r="AH1" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="AI1" s="30" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>8341026000105</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2">
+        <v>58113410</v>
+      </c>
+      <c r="G2">
+        <v>83998630647</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>299</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="L2" t="s">
+        <v>333</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" t="s">
+        <v>359</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q2">
+        <v>83998630647</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="S2" t="s">
+        <v>339</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>342</v>
+      </c>
+      <c r="V2">
+        <v>789</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="X2">
+        <v>898</v>
+      </c>
+      <c r="Y2">
+        <v>30</v>
+      </c>
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
+        <v>5</v>
+      </c>
+      <c r="AB2">
+        <v>9405591452</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>366</v>
+      </c>
+      <c r="AD2" s="20">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF2" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="AG2">
+        <v>83998630647</v>
+      </c>
+      <c r="AH2" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="AI2" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>8341026000105</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>300</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>305</v>
+      </c>
+      <c r="P3" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>343</v>
+      </c>
+      <c r="AD3" s="20">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>8341026000105</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>301</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>306</v>
+      </c>
+      <c r="P4" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>344</v>
+      </c>
+      <c r="AD4" s="20">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>8341026000105</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>302</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>307</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD5" s="20">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="20" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>308</v>
+      </c>
+      <c r="T6">
+        <v>5</v>
+      </c>
+      <c r="U6" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD6" s="20">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>309</v>
+      </c>
+      <c r="T7">
+        <v>6</v>
+      </c>
+      <c r="U7" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD7" s="20">
+        <v>6</v>
+      </c>
+      <c r="AE7" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8" t="s">
+        <v>292</v>
+      </c>
+      <c r="T8">
+        <v>7</v>
+      </c>
+      <c r="U8" t="s">
+        <v>302</v>
+      </c>
+      <c r="AD8" s="20">
+        <v>7</v>
+      </c>
+      <c r="AE8" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="M9" s="20">
+        <v>8</v>
+      </c>
+      <c r="N9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AD9" s="20">
+        <v>8</v>
+      </c>
+      <c r="AE9" s="20" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="M10" s="20">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>293</v>
+      </c>
+      <c r="AD10" s="20">
+        <v>9</v>
+      </c>
+      <c r="AE10" s="20" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="M11" s="20">
+        <v>10</v>
+      </c>
+      <c r="N11" t="s">
+        <v>311</v>
+      </c>
+      <c r="AD11" s="20">
+        <v>10</v>
+      </c>
+      <c r="AE11" s="20" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{6C6A87F7-8AA0-4D82-A4E4-5465F2853C90}"/>
+    <hyperlink ref="R2" r:id="rId2" xr:uid="{31680526-6A68-4BA6-BD6E-F8D5C2550A08}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{57E84587-75B2-4A52-81FE-D3E7E3696137}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{5A837180-0E10-4156-9C31-320507FFB5EB}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{A7EB4EE8-4114-4B78-B3C5-C8544D106967}"/>
+    <hyperlink ref="R3" r:id="rId6" xr:uid="{AA5EEA7D-313A-423D-BF9C-2C12FC661255}"/>
+    <hyperlink ref="R4" r:id="rId7" xr:uid="{8D75986E-B963-4B6F-B0A0-C9BFAF8D02FB}"/>
+    <hyperlink ref="R5" r:id="rId8" xr:uid="{EFDD48C7-604A-446B-A9DA-5F5EA9447870}"/>
+    <hyperlink ref="AH2" r:id="rId9" xr:uid="{89FF2193-DB6D-45E7-9EA3-D9004DF7BC6D}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adiconando cadastro da segregação de massa
</commit_message>
<xml_diff>
--- a/plano de amortização.xlsx
+++ b/plano de amortização.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F05A2-C297-4339-9235-014C4732C9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320F4A77-6E32-4E1A-8F09-8C9DC1756E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4755" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano_amortizacao vigente" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="423">
   <si>
     <t>ano</t>
   </si>
@@ -940,9 +940,6 @@
     <t>Vice-prefeito</t>
   </si>
   <si>
-    <t>da economia</t>
-  </si>
-  <si>
     <t>da cultura</t>
   </si>
   <si>
@@ -1042,9 +1039,6 @@
     <t>Cod_prev_compl</t>
   </si>
   <si>
-    <t>09405591452</t>
-  </si>
-  <si>
     <t>01/10/1999</t>
   </si>
   <si>
@@ -1147,9 +1141,6 @@
     <t xml:space="preserve">cod_natureza </t>
   </si>
   <si>
-    <t>06347458675</t>
-  </si>
-  <si>
     <t>05/05/2005</t>
   </si>
   <si>
@@ -1160,6 +1151,177 @@
   </si>
   <si>
     <t>31/12/2021</t>
+  </si>
+  <si>
+    <t>Toin do Gás</t>
+  </si>
+  <si>
+    <t>urtiotuieroute@hotmail.com</t>
+  </si>
+  <si>
+    <t>02/02/2026</t>
+  </si>
+  <si>
+    <t>vinculo</t>
+  </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>Autonomo</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Aposenta nois</t>
+  </si>
+  <si>
+    <t>Jardim</t>
+  </si>
+  <si>
+    <t>complemento</t>
+  </si>
+  <si>
+    <t>Bayeux</t>
+  </si>
+  <si>
+    <t>uteriou@gmail.com</t>
+  </si>
+  <si>
+    <t> AC</t>
+  </si>
+  <si>
+    <t> AL</t>
+  </si>
+  <si>
+    <t> AP</t>
+  </si>
+  <si>
+    <t> AM</t>
+  </si>
+  <si>
+    <t> BA</t>
+  </si>
+  <si>
+    <t> CE</t>
+  </si>
+  <si>
+    <t> DF</t>
+  </si>
+  <si>
+    <t> ES</t>
+  </si>
+  <si>
+    <t> GO</t>
+  </si>
+  <si>
+    <t> MA</t>
+  </si>
+  <si>
+    <t> MT</t>
+  </si>
+  <si>
+    <t> MS</t>
+  </si>
+  <si>
+    <t> MG</t>
+  </si>
+  <si>
+    <t> PA</t>
+  </si>
+  <si>
+    <t> PB</t>
+  </si>
+  <si>
+    <t> PR</t>
+  </si>
+  <si>
+    <t> PE</t>
+  </si>
+  <si>
+    <t> PI</t>
+  </si>
+  <si>
+    <t> RJ</t>
+  </si>
+  <si>
+    <t> RN</t>
+  </si>
+  <si>
+    <t> RS</t>
+  </si>
+  <si>
+    <t> RO</t>
+  </si>
+  <si>
+    <t> RR</t>
+  </si>
+  <si>
+    <t> SC</t>
+  </si>
+  <si>
+    <t> SP</t>
+  </si>
+  <si>
+    <t> SE</t>
+  </si>
+  <si>
+    <t> TO</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>58113-410</t>
+  </si>
+  <si>
+    <t>063.474.586-75</t>
+  </si>
+  <si>
+    <t>094.055.914-52</t>
+  </si>
+  <si>
+    <t>vendedor de inhame</t>
+  </si>
+  <si>
+    <t>vendedor de ovo</t>
+  </si>
+  <si>
+    <t>150.991.134-00</t>
+  </si>
+  <si>
+    <t>08398630647</t>
+  </si>
+  <si>
+    <t>art 5°</t>
+  </si>
+  <si>
+    <t>Segragação de massa</t>
+  </si>
+  <si>
+    <t>Não Possui</t>
+  </si>
+  <si>
+    <t>Instituída neste Exercício ou Mantida</t>
+  </si>
+  <si>
+    <t>Extinta neste Exercício</t>
+  </si>
+  <si>
+    <t>Revisada nesse Exercício</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>mant_tesouro_cívil</t>
+  </si>
+  <si>
+    <t>prv_compl</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1520,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1433,7 +1595,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hiperlink" xfId="6" builtinId="8"/>
@@ -2458,116 +2619,540 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4D80C-8621-48E7-94DF-8C2C1D847455}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="20" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="20" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="20"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="I1" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="P1" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="L1" t="s">
-        <v>271</v>
-      </c>
-      <c r="M1" t="s">
-        <v>272</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="V1" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="P1" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>276</v>
-      </c>
-      <c r="R1" t="s">
-        <v>275</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="W1" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="T1" t="s">
-        <v>323</v>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2">
+        <v>83998630647</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="E2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="G2" s="29">
+        <v>3</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="I2">
+        <v>789789</v>
+      </c>
+      <c r="J2">
+        <v>4546</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" t="s">
+        <v>373</v>
+      </c>
+      <c r="M2" t="s">
+        <v>284</v>
+      </c>
+      <c r="O2" t="s">
+        <v>374</v>
+      </c>
+      <c r="P2" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>378</v>
+      </c>
+      <c r="S2">
+        <v>58113410</v>
+      </c>
+      <c r="T2">
+        <v>83998630647</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q5" s="20">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q6" s="20">
+        <v>5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q7" s="20">
+        <v>6</v>
+      </c>
+      <c r="R7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q8" s="20">
+        <v>7</v>
+      </c>
+      <c r="R8" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="29"/>
+      <c r="Q9" s="20">
+        <v>8</v>
+      </c>
+      <c r="R9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q10" s="20">
+        <v>9</v>
+      </c>
+      <c r="R10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q11" s="20">
+        <v>10</v>
+      </c>
+      <c r="R11" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q12" s="20">
+        <v>11</v>
+      </c>
+      <c r="R12" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q13" s="20">
+        <v>12</v>
+      </c>
+      <c r="R13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q14" s="20">
+        <v>13</v>
+      </c>
+      <c r="R14" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q15" s="20">
+        <v>14</v>
+      </c>
+      <c r="R15" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q16" s="20">
+        <v>15</v>
+      </c>
+      <c r="R16" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="17" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q17" s="20">
+        <v>16</v>
+      </c>
+      <c r="R17" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="18" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q18" s="20">
+        <v>17</v>
+      </c>
+      <c r="R18" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="19" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q19" s="20">
+        <v>18</v>
+      </c>
+      <c r="R19" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="20" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q20" s="20">
+        <v>19</v>
+      </c>
+      <c r="R20" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q21" s="20">
+        <v>20</v>
+      </c>
+      <c r="R21" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="22" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q22" s="20">
+        <v>21</v>
+      </c>
+      <c r="R22" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="23" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q23" s="20">
+        <v>22</v>
+      </c>
+      <c r="R23" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="24" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q24" s="20">
+        <v>23</v>
+      </c>
+      <c r="R24" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q25" s="20">
+        <v>24</v>
+      </c>
+      <c r="R25" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="26" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q26" s="20">
+        <v>25</v>
+      </c>
+      <c r="R26" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="27" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q27" s="20">
+        <v>26</v>
+      </c>
+      <c r="R27" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="28" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q28" s="20">
+        <v>27</v>
+      </c>
+      <c r="R28" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4F52068C-10C9-439D-BC73-19AE05EDE30C}"/>
+    <hyperlink ref="U2" r:id="rId2" xr:uid="{DEA32A72-2D18-49A4-9263-23E6FA5A89DA}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC23F32-023E-4679-8D32-C792213F62D3}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>414</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="B1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="G1" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="I1" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="E1" t="s">
-        <v>328</v>
+      <c r="J1" s="30" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="20">
+        <v>1</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="I2" s="20">
+        <v>1</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="20">
+        <v>2</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="I3" s="20">
+        <v>2</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -4441,7 +5026,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6579,65 +7164,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1491B68-B113-4854-8907-E7E5C981C4E4}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>271</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="30" t="s">
         <v>274</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="30" t="s">
         <v>279</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="30" t="s">
         <v>283</v>
       </c>
     </row>
@@ -6654,14 +7237,14 @@
       <c r="D2">
         <v>58113410</v>
       </c>
-      <c r="E2">
-        <v>83998630647</v>
+      <c r="E2" s="29" t="s">
+        <v>412</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>287</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
       <c r="H2" t="s">
         <v>288</v>
@@ -6673,13 +7256,13 @@
         <v>292</v>
       </c>
       <c r="K2" t="s">
-        <v>295</v>
+        <v>409</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6695,14 +7278,14 @@
       <c r="D3" s="20">
         <v>58113410</v>
       </c>
-      <c r="E3" s="20">
-        <v>83998630647</v>
+      <c r="E3" s="29" t="s">
+        <v>412</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>287</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>288</v>
@@ -6714,10 +7297,10 @@
         <v>291</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -6733,14 +7316,14 @@
       <c r="D4" s="20">
         <v>58113410</v>
       </c>
-      <c r="E4" s="20">
-        <v>83998630647</v>
+      <c r="E4" s="29" t="s">
+        <v>412</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>287</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>288</v>
@@ -6752,10 +7335,10 @@
         <v>290</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6771,14 +7354,14 @@
       <c r="D5" s="20">
         <v>58113410</v>
       </c>
-      <c r="E5" s="20">
-        <v>83998630647</v>
+      <c r="E5" s="29" t="s">
+        <v>412</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>287</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>288</v>
@@ -6790,13 +7373,13 @@
         <v>293</v>
       </c>
       <c r="K5" t="s">
+        <v>295</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="M5" s="26" t="s">
         <v>296</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>330</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -6812,14 +7395,14 @@
       <c r="D6" s="20">
         <v>58113410</v>
       </c>
-      <c r="E6" s="20">
-        <v>83998630647</v>
+      <c r="E6" s="29" t="s">
+        <v>412</v>
       </c>
       <c r="F6" s="26" t="s">
         <v>287</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>288</v>
@@ -6831,10 +7414,10 @@
         <v>294</v>
       </c>
       <c r="L6" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M6" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -6853,11 +7436,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB190852-2510-45CC-A5C2-C7FDFE63385C}">
-  <dimension ref="A1:AI11"/>
+  <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
-    </sheetView>
+    <sheetView topLeftCell="AB1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6871,44 +7452,45 @@
     <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.28515625" style="20" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.28515625" style="20" customWidth="1"/>
+    <col min="34" max="34" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>130</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>271</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>273</v>
       </c>
       <c r="E1" s="30" t="s">
@@ -6918,96 +7500,99 @@
         <v>274</v>
       </c>
       <c r="G1" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>361</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="S1" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="H1" s="30" t="s">
-        <v>335</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>363</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="L1" s="30" t="s">
+      <c r="T1" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="V1" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="W1" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="X1" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="Y1" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="Z1" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="AA1" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="AB1" s="31" t="s">
+        <v>351</v>
+      </c>
+      <c r="AC1" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="AD1" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="M1" s="30" t="s">
-        <v>303</v>
-      </c>
-      <c r="N1" s="30" t="s">
+      <c r="AE1" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="AF1" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="O1" s="31" t="s">
-        <v>361</v>
-      </c>
-      <c r="P1" s="30" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q1" s="30" t="s">
-        <v>337</v>
-      </c>
-      <c r="R1" s="30" t="s">
-        <v>338</v>
-      </c>
-      <c r="S1" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="T1" s="30" t="s">
-        <v>340</v>
-      </c>
-      <c r="U1" s="30" t="s">
-        <v>341</v>
-      </c>
-      <c r="V1" s="30" t="s">
-        <v>348</v>
-      </c>
-      <c r="W1" s="30" t="s">
-        <v>349</v>
-      </c>
-      <c r="X1" s="30" t="s">
-        <v>350</v>
-      </c>
-      <c r="Y1" s="30" t="s">
-        <v>351</v>
-      </c>
-      <c r="Z1" s="30" t="s">
-        <v>352</v>
-      </c>
-      <c r="AA1" s="30" t="s">
+      <c r="AG1" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="AH1" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AI1" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="AC1" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="AD1" s="30" t="s">
-        <v>303</v>
-      </c>
-      <c r="AE1" s="30" t="s">
-        <v>289</v>
-      </c>
-      <c r="AF1" s="30" t="s">
-        <v>273</v>
-      </c>
-      <c r="AG1" s="30" t="s">
+      <c r="AJ1" s="30" t="s">
         <v>355</v>
       </c>
-      <c r="AH1" s="30" t="s">
-        <v>356</v>
-      </c>
-      <c r="AI1" s="30" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
-        <v>8341026000105</v>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>177</v>
@@ -7018,100 +7603,103 @@
       <c r="E2" t="s">
         <v>286</v>
       </c>
-      <c r="F2">
-        <v>58113410</v>
+      <c r="F2" t="s">
+        <v>406</v>
       </c>
       <c r="G2">
         <v>83998630647</v>
       </c>
       <c r="H2" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="I2" s="20">
+        <v>4</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>407</v>
+      </c>
+      <c r="M2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>303</v>
+      </c>
+      <c r="P2" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q2" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="R2">
+        <v>83998630647</v>
+      </c>
+      <c r="S2" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>299</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>364</v>
-      </c>
-      <c r="L2" t="s">
-        <v>333</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>304</v>
-      </c>
-      <c r="O2" t="s">
-        <v>359</v>
-      </c>
-      <c r="P2" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q2">
-        <v>83998630647</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="S2" t="s">
-        <v>339</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
-        <v>342</v>
-      </c>
-      <c r="V2">
+      <c r="T2" t="s">
+        <v>337</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>340</v>
+      </c>
+      <c r="W2">
         <v>789</v>
       </c>
-      <c r="W2" s="19" t="s">
-        <v>358</v>
-      </c>
-      <c r="X2">
+      <c r="X2" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="Y2">
         <v>898</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>30</v>
-      </c>
-      <c r="Z2">
-        <v>5</v>
       </c>
       <c r="AA2">
         <v>5</v>
       </c>
-      <c r="AB2">
-        <v>9405591452</v>
+      <c r="AB2" t="s">
+        <v>413</v>
       </c>
       <c r="AC2" t="s">
-        <v>366</v>
-      </c>
-      <c r="AD2" s="20">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="20" t="s">
-        <v>304</v>
+        <v>408</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE2" s="20">
+        <v>1</v>
       </c>
       <c r="AF2" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="AG2">
+        <v>303</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="AH2">
         <v>83998630647</v>
       </c>
-      <c r="AH2" s="26" t="s">
-        <v>360</v>
-      </c>
-      <c r="AI2" s="28" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
-        <v>8341026000105</v>
+      <c r="AI2" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="AJ2" s="28" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>177</v>
@@ -7120,7 +7708,7 @@
         <v>284</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>286</v>
@@ -7130,48 +7718,48 @@
         <v>83998630647</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>300</v>
-      </c>
-      <c r="M3">
+        <v>299</v>
+      </c>
+      <c r="N3">
         <v>2</v>
       </c>
-      <c r="N3" t="s">
-        <v>305</v>
-      </c>
-      <c r="P3" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q3" s="20">
+      <c r="O3" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="R3" s="20">
         <v>83998630647</v>
       </c>
-      <c r="R3" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="S3" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="T3">
+      <c r="S3" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="U3">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
-        <v>343</v>
-      </c>
-      <c r="AD3" s="20">
+      <c r="V3" t="s">
+        <v>341</v>
+      </c>
+      <c r="AE3" s="20">
         <v>2</v>
       </c>
-      <c r="AE3" s="20" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
-        <v>8341026000105</v>
+      <c r="AF3" s="20" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>177</v>
@@ -7180,7 +7768,7 @@
         <v>284</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>286</v>
@@ -7190,48 +7778,48 @@
         <v>83998630647</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>301</v>
-      </c>
-      <c r="M4">
+        <v>300</v>
+      </c>
+      <c r="N4">
         <v>3</v>
       </c>
-      <c r="N4" t="s">
-        <v>306</v>
-      </c>
-      <c r="P4" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q4" s="20">
+      <c r="O4" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="R4" s="20">
         <v>83998630647</v>
       </c>
-      <c r="R4" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="T4">
+      <c r="S4" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="U4">
         <v>3</v>
       </c>
-      <c r="U4" t="s">
-        <v>344</v>
-      </c>
-      <c r="AD4" s="20">
+      <c r="V4" t="s">
+        <v>342</v>
+      </c>
+      <c r="AE4" s="20">
         <v>3</v>
       </c>
-      <c r="AE4" s="20" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
-        <v>8341026000105</v>
+      <c r="AF4" s="20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>177</v>
@@ -7240,7 +7828,7 @@
         <v>284</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>286</v>
@@ -7250,159 +7838,160 @@
         <v>83998630647</v>
       </c>
       <c r="H5" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>298</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="R5" s="20">
+        <v>83998630647</v>
+      </c>
+      <c r="S5" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="I5">
+      <c r="T5" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="U5">
         <v>4</v>
       </c>
-      <c r="J5" t="s">
-        <v>302</v>
-      </c>
-      <c r="M5">
+      <c r="V5" t="s">
+        <v>343</v>
+      </c>
+      <c r="AE5" s="20">
         <v>4</v>
       </c>
-      <c r="N5" t="s">
+      <c r="AF5" s="20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
         <v>307</v>
       </c>
-      <c r="P5" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q5" s="20">
-        <v>83998630647</v>
-      </c>
-      <c r="R5" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="T5">
-        <v>4</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="V6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AE6" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF6" s="20" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
+        <v>308</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7" t="s">
         <v>345</v>
       </c>
-      <c r="AD5" s="20">
-        <v>4</v>
-      </c>
-      <c r="AE5" s="20" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M6">
-        <v>5</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="AE7" s="20">
+        <v>6</v>
+      </c>
+      <c r="AF7" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="T6">
-        <v>5</v>
-      </c>
-      <c r="U6" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD6" s="20">
-        <v>5</v>
-      </c>
-      <c r="AE6" s="20" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M7">
-        <v>6</v>
-      </c>
-      <c r="N7" t="s">
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8" t="s">
+        <v>292</v>
+      </c>
+      <c r="U8">
+        <v>7</v>
+      </c>
+      <c r="V8" t="s">
+        <v>301</v>
+      </c>
+      <c r="AE8" s="20">
+        <v>7</v>
+      </c>
+      <c r="AF8" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="N9" s="20">
+        <v>8</v>
+      </c>
+      <c r="O9" t="s">
         <v>309</v>
       </c>
-      <c r="T7">
-        <v>6</v>
-      </c>
-      <c r="U7" t="s">
-        <v>347</v>
-      </c>
-      <c r="AD7" s="20">
-        <v>6</v>
-      </c>
-      <c r="AE7" s="20" t="s">
+      <c r="AE9" s="20">
+        <v>8</v>
+      </c>
+      <c r="AF9" s="20" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M8">
-        <v>7</v>
-      </c>
-      <c r="N8" t="s">
-        <v>292</v>
-      </c>
-      <c r="T8">
-        <v>7</v>
-      </c>
-      <c r="U8" t="s">
-        <v>302</v>
-      </c>
-      <c r="AD8" s="20">
-        <v>7</v>
-      </c>
-      <c r="AE8" s="20" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M9" s="20">
-        <v>8</v>
-      </c>
-      <c r="N9" t="s">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="N10" s="20">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>293</v>
+      </c>
+      <c r="AE10" s="20">
+        <v>9</v>
+      </c>
+      <c r="AF10" s="20" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="N11" s="20">
+        <v>10</v>
+      </c>
+      <c r="O11" t="s">
         <v>310</v>
       </c>
-      <c r="AD9" s="20">
-        <v>8</v>
-      </c>
-      <c r="AE9" s="20" t="s">
+      <c r="AE11" s="20">
+        <v>10</v>
+      </c>
+      <c r="AF11" s="20" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M10" s="20">
-        <v>9</v>
-      </c>
-      <c r="N10" t="s">
-        <v>293</v>
-      </c>
-      <c r="AD10" s="20">
-        <v>9</v>
-      </c>
-      <c r="AE10" s="20" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M11" s="20">
-        <v>10</v>
-      </c>
-      <c r="N11" t="s">
-        <v>311</v>
-      </c>
-      <c r="AD11" s="20">
-        <v>10</v>
-      </c>
-      <c r="AE11" s="20" t="s">
-        <v>311</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{6C6A87F7-8AA0-4D82-A4E4-5465F2853C90}"/>
-    <hyperlink ref="R2" r:id="rId2" xr:uid="{31680526-6A68-4BA6-BD6E-F8D5C2550A08}"/>
+    <hyperlink ref="S2" r:id="rId2" xr:uid="{31680526-6A68-4BA6-BD6E-F8D5C2550A08}"/>
     <hyperlink ref="H3" r:id="rId3" xr:uid="{57E84587-75B2-4A52-81FE-D3E7E3696137}"/>
     <hyperlink ref="H4" r:id="rId4" xr:uid="{5A837180-0E10-4156-9C31-320507FFB5EB}"/>
     <hyperlink ref="H5" r:id="rId5" xr:uid="{A7EB4EE8-4114-4B78-B3C5-C8544D106967}"/>
-    <hyperlink ref="R3" r:id="rId6" xr:uid="{AA5EEA7D-313A-423D-BF9C-2C12FC661255}"/>
-    <hyperlink ref="R4" r:id="rId7" xr:uid="{8D75986E-B963-4B6F-B0A0-C9BFAF8D02FB}"/>
-    <hyperlink ref="R5" r:id="rId8" xr:uid="{EFDD48C7-604A-446B-A9DA-5F5EA9447870}"/>
-    <hyperlink ref="AH2" r:id="rId9" xr:uid="{89FF2193-DB6D-45E7-9EA3-D9004DF7BC6D}"/>
+    <hyperlink ref="S3" r:id="rId6" xr:uid="{AA5EEA7D-313A-423D-BF9C-2C12FC661255}"/>
+    <hyperlink ref="S4" r:id="rId7" xr:uid="{8D75986E-B963-4B6F-B0A0-C9BFAF8D02FB}"/>
+    <hyperlink ref="S5" r:id="rId8" xr:uid="{EFDD48C7-604A-446B-A9DA-5F5EA9447870}"/>
+    <hyperlink ref="AI2" r:id="rId9" xr:uid="{89FF2193-DB6D-45E7-9EA3-D9004DF7BC6D}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
parte do cadastro dos militares
</commit_message>
<xml_diff>
--- a/plano de amortização.xlsx
+++ b/plano de amortização.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320F4A77-6E32-4E1A-8F09-8C9DC1756E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C04655-3360-4527-98E7-C0968D771F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano_amortizacao vigente" sheetId="2" r:id="rId1"/>
@@ -24,9 +24,11 @@
     <sheet name="UG" sheetId="9" r:id="rId9"/>
     <sheet name="Atuário" sheetId="10" r:id="rId10"/>
     <sheet name="Composição de massa" sheetId="11" r:id="rId11"/>
+    <sheet name="Militar prev-val compromissos " sheetId="13" r:id="rId12"/>
+    <sheet name="Militar-com-proj-exe" sheetId="14" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Modelo DRAA Precificador'!$A$1:$N$11</definedName>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="424">
   <si>
     <t>ano</t>
   </si>
@@ -1322,6 +1324,9 @@
   </si>
   <si>
     <t>prv_compl</t>
+  </si>
+  <si>
+    <t>Geração Futura</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1399,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1446,6 +1451,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1520,7 +1531,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1595,6 +1606,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="10" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hiperlink" xfId="6" builtinId="8"/>
@@ -2048,10 +2065,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EBBB80-D39B-4C5D-8A0E-1203E2F98462}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,10 +2639,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4D80C-8621-48E7-94DF-8C2C1D847455}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3012,10 +3035,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC23F32-023E-4679-8D32-C792213F62D3}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3160,12 +3186,961 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63515ED-F71D-4E41-8A65-2B8BF3B4D2A6}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="113.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11">
+        <v>372140643629</v>
+      </c>
+      <c r="C2" s="33">
+        <v>11111111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="11">
+        <v>111111111</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="11">
+        <v>222222222</v>
+      </c>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="11">
+        <v>333333333</v>
+      </c>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11">
+        <v>4444444444444</v>
+      </c>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="11">
+        <v>55555555555555</v>
+      </c>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="11">
+        <v>5689742597</v>
+      </c>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="11">
+        <v>362119589.00000006</v>
+      </c>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="11">
+        <v>2018465488</v>
+      </c>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1111111111</v>
+      </c>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="11">
+        <v>2222222222</v>
+      </c>
+      <c r="C15" s="13"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="11">
+        <v>4444444444</v>
+      </c>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="11">
+        <v>5555555555</v>
+      </c>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="11">
+        <v>20615686</v>
+      </c>
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="11">
+        <v>109098327</v>
+      </c>
+      <c r="C20" s="13"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="11">
+        <v>11111111111111</v>
+      </c>
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="11">
+        <v>74592946760</v>
+      </c>
+      <c r="C24" s="11">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="11">
+        <v>58900728662</v>
+      </c>
+      <c r="C25" s="11">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="11">
+        <v>4829853727</v>
+      </c>
+      <c r="C26" s="11">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="11">
+        <v>1111111111111</v>
+      </c>
+      <c r="C27" s="11">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="11">
+        <v>222222222222</v>
+      </c>
+      <c r="C28" s="11">
+        <v>55555555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="11">
+        <v>19175652023</v>
+      </c>
+      <c r="C29" s="11">
+        <v>66666666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="11">
+        <v>3333333333</v>
+      </c>
+      <c r="C30" s="11">
+        <v>77777777</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="11">
+        <v>4444444444444</v>
+      </c>
+      <c r="C31" s="11">
+        <v>88888888</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="11">
+        <v>64560199325.999985</v>
+      </c>
+      <c r="C33" s="11">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="11">
+        <v>46114428088</v>
+      </c>
+      <c r="C34" s="11">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="11">
+        <v>278414128</v>
+      </c>
+      <c r="C35" s="11">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="11">
+        <v>44431534</v>
+      </c>
+      <c r="C36" s="11">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="11">
+        <v>12599934494</v>
+      </c>
+      <c r="C37" s="11">
+        <v>55555555</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="33">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="15"/>
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="16">
+        <v>898998089</v>
+      </c>
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="16">
+        <v>78978562623</v>
+      </c>
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="14"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="32"/>
+      <c r="C49" s="14"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="32"/>
+      <c r="C50" s="14"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="16">
+        <v>222222222222222</v>
+      </c>
+      <c r="C51" s="14"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="32"/>
+      <c r="C52" s="14"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="32"/>
+      <c r="C53" s="14"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="16">
+        <v>555555555555</v>
+      </c>
+      <c r="C54" s="14"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="16">
+        <v>7897484546</v>
+      </c>
+      <c r="C55" s="14"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="32"/>
+      <c r="C56" s="14"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="16">
+        <v>4444444444444</v>
+      </c>
+      <c r="C57" s="14"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="16">
+        <v>555555555555</v>
+      </c>
+      <c r="C58" s="14"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" s="32"/>
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="32"/>
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="32"/>
+      <c r="C61" s="14"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" s="32"/>
+      <c r="C62" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD749E82-367C-4624-B4A9-EF534CA8D9DC}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="24">
+        <v>1111111</v>
+      </c>
+      <c r="C2" s="24">
+        <v>1388888.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="24">
+        <v>2222222</v>
+      </c>
+      <c r="C3" s="24">
+        <v>2777777.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="24">
+        <v>3333333</v>
+      </c>
+      <c r="C4" s="24">
+        <v>4166666.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="24">
+        <v>4444444</v>
+      </c>
+      <c r="C5" s="24">
+        <v>5555555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="24">
+        <v>5555555</v>
+      </c>
+      <c r="C6" s="24">
+        <v>6944443.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="24">
+        <v>6666666</v>
+      </c>
+      <c r="C7" s="24">
+        <v>8333332.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="24">
+        <v>7777777</v>
+      </c>
+      <c r="C8" s="24">
+        <v>9722221.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="24">
+        <v>8888888</v>
+      </c>
+      <c r="C9" s="24">
+        <v>11111110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="24">
+        <v>999999</v>
+      </c>
+      <c r="C10" s="24">
+        <v>1249998.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" s="24">
+        <v>10101010</v>
+      </c>
+      <c r="C11" s="24">
+        <v>12626262.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" s="24">
+        <v>1111111111</v>
+      </c>
+      <c r="C12" s="24">
+        <v>1388888888.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="24">
+        <v>9597874415</v>
+      </c>
+      <c r="C13" s="24">
+        <v>11997343018.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" s="24">
+        <v>1111111</v>
+      </c>
+      <c r="C14" s="24">
+        <v>6057648205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15" s="24">
+        <v>2222222</v>
+      </c>
+      <c r="C15" s="24">
+        <v>605605205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" s="24">
+        <v>3333333</v>
+      </c>
+      <c r="C16" s="24">
+        <v>60570608080</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="24">
+        <v>4444444</v>
+      </c>
+      <c r="C17" s="24">
+        <v>6061449560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="24">
+        <v>5555555</v>
+      </c>
+      <c r="C18" s="24">
+        <v>6116617789</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="24">
+        <v>6666666</v>
+      </c>
+      <c r="C19" s="24">
+        <v>1119610820</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B20" s="24">
+        <v>7777777</v>
+      </c>
+      <c r="C20" s="24">
+        <v>18290530625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="24">
+        <v>8888888</v>
+      </c>
+      <c r="C21" s="24">
+        <v>858206.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" s="24">
+        <v>999999</v>
+      </c>
+      <c r="C22" s="24">
+        <v>12373695</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" s="24">
+        <v>10101010</v>
+      </c>
+      <c r="C23" s="24">
+        <v>373210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B24" s="24">
+        <v>1111111111</v>
+      </c>
+      <c r="C24" s="24">
+        <v>4484973.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B25" s="24">
+        <v>121211222</v>
+      </c>
+      <c r="C25" s="24">
+        <v>1098070231.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B26" s="24">
+        <v>13131313</v>
+      </c>
+      <c r="C26" s="24">
+        <v>4961243.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B27" s="24">
+        <v>1414141414</v>
+      </c>
+      <c r="C27" s="24">
+        <v>85573181.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B28" s="24">
+        <v>15151515155</v>
+      </c>
+      <c r="C28" s="24">
+        <v>1098318317.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B29" s="24">
+        <v>161616161</v>
+      </c>
+      <c r="C29" s="24">
+        <v>935956445</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B30" s="24">
+        <v>78455615</v>
+      </c>
+      <c r="C30" s="24">
+        <v>98069518.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B31" s="24">
+        <v>24848948</v>
+      </c>
+      <c r="C31" s="24">
+        <v>31061185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B32" s="24">
+        <v>1846487</v>
+      </c>
+      <c r="C32" s="24">
+        <v>2308108.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B33" s="24">
+        <v>7479876</v>
+      </c>
+      <c r="C33" s="24">
+        <v>9349845</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3809,10 +4784,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF10D5-ABDD-4F59-8C94-2B7C746ACA7C}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4468,10 +5446,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F764EF3B-304D-4F9A-AF09-04DC8A7C5C52}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5023,10 +6004,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710037F9-F9A9-4156-B689-1E1185376461}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5908,10 +6892,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4DAA86-620B-43A7-A1AB-8BB9B378D86A}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6747,10 +7734,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737DF4F8-5AC6-4CD3-A777-EBE20E8E4EAD}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7162,9 +8152,14 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1491B68-B113-4854-8907-E7E5C981C4E4}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7436,9 +8431,14 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB190852-2510-45CC-A5C2-C7FDFE63385C}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>